<commit_message>
update schema diagram & db spread sheet
</commit_message>
<xml_diff>
--- a/Database Design.xlsx
+++ b/Database Design.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NTU\Module 3\project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\linux\NTU\SCTP Java Projects\Library-Booking-System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24860783-46DB-4442-AD09-642FDBF3F432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{724ADFCD-4B7E-4DA5-A584-918D1F1825A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{3DD5B3BD-22E3-4A62-824F-9C319636EE68}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
   <si>
     <t>title</t>
   </si>
@@ -42,12 +42,6 @@
     <t>availability</t>
   </si>
   <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
@@ -103,12 +97,6 @@
   </si>
   <si>
     <t>loan_period</t>
-  </si>
-  <si>
-    <t>books</t>
-  </si>
-  <si>
-    <t>users</t>
   </si>
   <si>
     <t>starttime</t>
@@ -188,6 +176,36 @@
       </rPr>
       <t>(ENUM)</t>
     </r>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>learner_firstname</t>
+  </si>
+  <si>
+    <t>learner_lastname</t>
+  </si>
+  <si>
+    <t>book_title</t>
+  </si>
+  <si>
+    <t>GHI</t>
+  </si>
+  <si>
+    <t>UserC</t>
+  </si>
+  <si>
+    <t>learner</t>
+  </si>
+  <si>
+    <t>book</t>
+  </si>
+  <si>
+    <t>contact_no</t>
   </si>
 </sst>
 </file>
@@ -225,7 +243,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -285,11 +303,78 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -309,9 +394,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -321,6 +403,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -635,45 +729,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63C35378-52BD-467A-A0B4-65DBC921DDC7}">
-  <dimension ref="B1:O14"/>
+  <dimension ref="B1:Q14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="4.26953125" customWidth="1"/>
     <col min="3" max="3" width="10.1796875" customWidth="1"/>
     <col min="4" max="4" width="10.36328125" customWidth="1"/>
     <col min="5" max="5" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.54296875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.6328125" customWidth="1"/>
-    <col min="11" max="11" width="12.26953125" customWidth="1"/>
-    <col min="12" max="12" width="12.81640625" customWidth="1"/>
-    <col min="15" max="15" width="17.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.81640625" customWidth="1"/>
+    <col min="10" max="10" width="12.26953125" customWidth="1"/>
+    <col min="11" max="12" width="12.81640625" customWidth="1"/>
+    <col min="13" max="13" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:17" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="6" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
-      <c r="J2" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="10"/>
-    </row>
-    <row r="3" spans="2:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="9"/>
+    </row>
+    <row r="3" spans="2:17" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>0</v>
@@ -690,37 +792,46 @@
       <c r="G3" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="I3" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="J3" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="L3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="N3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="O3" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="2:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="O3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="2:17" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="1">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F4" s="1">
         <v>1</v>
@@ -728,81 +839,102 @@
       <c r="G4" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="I4" s="1">
+        <v>1</v>
+      </c>
       <c r="J4" s="1">
         <v>1</v>
       </c>
       <c r="K4" s="1">
-        <v>1</v>
-      </c>
-      <c r="L4" s="1">
         <v>2</v>
       </c>
-      <c r="M4" s="3">
+      <c r="L4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O4" s="3">
         <v>45265</v>
       </c>
-      <c r="N4" s="3">
+      <c r="P4" s="3">
         <v>45268</v>
       </c>
-      <c r="O4" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="2:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="Q4" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="1">
         <v>2</v>
       </c>
-      <c r="C5" s="1">
-        <v>123</v>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" s="1">
+        <v>2</v>
+      </c>
+      <c r="J5" s="1">
+        <v>1</v>
+      </c>
+      <c r="K5" s="1">
+        <v>1</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="1">
-        <v>1</v>
-      </c>
-      <c r="G5" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="J5" s="1">
-        <v>2</v>
-      </c>
-      <c r="K5" s="1">
-        <v>1</v>
-      </c>
-      <c r="L5" s="1">
-        <v>1</v>
-      </c>
-      <c r="M5" s="3">
+      <c r="N5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O5" s="3">
         <v>45265</v>
       </c>
-      <c r="N5" s="3">
+      <c r="P5" s="3">
         <v>45268</v>
       </c>
-      <c r="O5" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="2:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="Q5" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6" s="1">
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F6" s="1">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="I6" s="1">
+        <v>3</v>
       </c>
       <c r="J6" s="1">
         <v>3</v>
@@ -810,98 +942,123 @@
       <c r="K6" s="1">
         <v>3</v>
       </c>
-      <c r="L6" s="1">
-        <v>3</v>
-      </c>
-      <c r="M6" s="3">
+      <c r="L6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O6" s="3">
         <v>45262</v>
       </c>
-      <c r="N6" s="3">
+      <c r="P6" s="3">
         <v>45265</v>
       </c>
-      <c r="O6" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="2:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="Q6" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
-      <c r="O7" s="2"/>
-    </row>
-    <row r="8" spans="2:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="9" spans="2:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-    </row>
-    <row r="10" spans="2:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="5" t="s">
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="2"/>
+    </row>
+    <row r="8" spans="2:17" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F8" s="11"/>
+    </row>
+    <row r="9" spans="2:17" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="12"/>
+    </row>
+    <row r="10" spans="2:17" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="D10" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="2:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="11" spans="2:17" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="5">
         <v>1</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="2:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>17</v>
+      </c>
+      <c r="E11" s="5">
+        <v>91234567</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B12" s="5">
         <v>2</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="2:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>18</v>
+      </c>
+      <c r="E12" s="5">
+        <v>923456789</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B13" s="5">
         <v>3</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="2:15" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+        <v>19</v>
+      </c>
+      <c r="E13" s="5">
+        <v>934567890</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="J2:O2"/>
+    <mergeCell ref="I2:Q2"/>
+    <mergeCell ref="B9:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>